<commit_message>
fix(import_devices): testing imported devices and fixing errors
</commit_message>
<xml_diff>
--- a/server/static/download/templates/devices_template_en.xlsx
+++ b/server/static/download/templates/devices_template_en.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>deviceName</t>
   </si>
@@ -27,9 +27,6 @@
   </si>
   <si>
     <t>IMEI</t>
-  </si>
-  <si>
-    <t>modBusIndex</t>
   </si>
   <si>
     <t>gateway</t>
@@ -86,9 +83,6 @@
   </si>
   <si>
     <t>Required only for LwM2M</t>
-  </si>
-  <si>
-    <t>Must a number between 0 and 255,only for Modus</t>
   </si>
   <si>
     <t>Gateway name,required only for upLinkSystem is gateway</t>
@@ -120,9 +114,6 @@
     <t>381787278348467</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>sample gateway</t>
   </si>
   <si>
@@ -141,7 +132,7 @@
     <t xml:space="preserve">sample row </t>
   </si>
   <si>
-    <t>0/1</t>
+    <t>1</t>
   </si>
   <si>
     <r>
@@ -416,7 +407,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -425,9 +416,6 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -1553,7 +1541,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1563,14 +1551,14 @@
     <col min="2" max="2" width="16.3516" style="1" customWidth="1"/>
     <col min="3" max="4" width="31" style="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="1" customWidth="1"/>
-    <col min="6" max="8" width="33" style="1" customWidth="1"/>
-    <col min="9" max="9" width="33.3516" style="1" customWidth="1"/>
-    <col min="10" max="10" width="34.1719" style="1" customWidth="1"/>
-    <col min="11" max="12" width="16.3516" style="1" customWidth="1"/>
-    <col min="13" max="16" width="20.5" style="1" customWidth="1"/>
-    <col min="17" max="17" width="21" style="1" customWidth="1"/>
-    <col min="18" max="19" width="16.3516" style="1" customWidth="1"/>
-    <col min="20" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="6" max="7" width="33" style="1" customWidth="1"/>
+    <col min="8" max="8" width="33.3516" style="1" customWidth="1"/>
+    <col min="9" max="9" width="34.1719" style="1" customWidth="1"/>
+    <col min="10" max="11" width="16.3516" style="1" customWidth="1"/>
+    <col min="12" max="15" width="20.5" style="1" customWidth="1"/>
+    <col min="16" max="16" width="21" style="1" customWidth="1"/>
+    <col min="17" max="18" width="16.3516" style="1" customWidth="1"/>
+    <col min="19" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1592,348 +1580,330 @@
       <c r="F1" t="s" s="3">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="4">
+      <c r="G1" t="s" s="3">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="4">
+      <c r="H1" t="s" s="3">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="4">
+      <c r="I1" t="s" s="3">
         <v>8</v>
       </c>
       <c r="J1" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="5">
+      <c r="K1" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="5">
+      <c r="L1" t="s" s="4">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="5">
+      <c r="M1" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="N1" t="s" s="5">
+      <c r="N1" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="O1" t="s" s="5">
+      <c r="O1" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="P1" t="s" s="5">
+      <c r="P1" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="Q1" t="s" s="5">
+      <c r="Q1" t="s" s="4">
         <v>16</v>
       </c>
-      <c r="R1" t="s" s="5">
+      <c r="R1" t="s" s="4">
         <v>17</v>
-      </c>
-      <c r="S1" t="s" s="5">
-        <v>18</v>
       </c>
     </row>
     <row r="2" ht="77" customHeight="1">
-      <c r="A2" t="s" s="6">
+      <c r="A2" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s" s="5">
         <v>19</v>
       </c>
-      <c r="B2" t="s" s="6">
+      <c r="C2" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="D2" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="D2" t="s" s="6">
+      <c r="E2" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="E2" t="s" s="6">
+      <c r="F2" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="F2" t="s" s="6">
+      <c r="G2" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="G2" t="s" s="6">
+      <c r="H2" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s" s="5">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s" s="5">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="Q2" t="s" s="5">
         <v>25</v>
       </c>
-      <c r="H2" t="s" s="6">
+      <c r="R2" t="s" s="5">
         <v>26</v>
-      </c>
-      <c r="I2" t="s" s="6">
-        <v>26</v>
-      </c>
-      <c r="J2" t="s" s="6">
-        <v>26</v>
-      </c>
-      <c r="K2" t="s" s="6">
-        <v>10</v>
-      </c>
-      <c r="L2" t="s" s="6">
-        <v>11</v>
-      </c>
-      <c r="M2" t="s" s="6">
-        <v>12</v>
-      </c>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" t="s" s="6">
-        <v>26</v>
-      </c>
-      <c r="R2" t="s" s="6">
-        <v>27</v>
-      </c>
-      <c r="S2" t="s" s="6">
-        <v>28</v>
       </c>
     </row>
     <row r="3" ht="20" customHeight="1">
-      <c r="A3" t="s" s="8">
+      <c r="A3" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s" s="8">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s" s="8">
         <v>29</v>
       </c>
-      <c r="B3" t="s" s="9">
+      <c r="D3" t="s" s="8">
         <v>30</v>
       </c>
-      <c r="C3" t="s" s="9">
+      <c r="E3" t="s" s="8">
         <v>31</v>
       </c>
-      <c r="D3" t="s" s="9">
+      <c r="F3" t="s" s="8">
         <v>32</v>
       </c>
-      <c r="E3" t="s" s="9">
+      <c r="G3" t="s" s="8">
         <v>33</v>
       </c>
-      <c r="F3" t="s" s="9">
+      <c r="H3" t="s" s="8">
+        <v>33</v>
+      </c>
+      <c r="I3" t="s" s="8">
+        <v>33</v>
+      </c>
+      <c r="J3" s="9">
+        <v>116.868765448363</v>
+      </c>
+      <c r="K3" s="9">
+        <v>24.4990810465301</v>
+      </c>
+      <c r="L3" t="s" s="8">
         <v>34</v>
       </c>
-      <c r="G3" t="s" s="9">
+      <c r="M3" t="s" s="8">
         <v>35</v>
       </c>
-      <c r="H3" t="s" s="9">
+      <c r="N3" t="s" s="8">
+        <v>35</v>
+      </c>
+      <c r="O3" t="s" s="8">
         <v>36</v>
       </c>
-      <c r="I3" t="s" s="9">
-        <v>36</v>
-      </c>
-      <c r="J3" t="s" s="9">
-        <v>36</v>
-      </c>
-      <c r="K3" s="10">
-        <v>116.868765448363</v>
-      </c>
-      <c r="L3" s="10">
-        <v>24.4990810465301</v>
-      </c>
-      <c r="M3" t="s" s="9">
+      <c r="P3" t="s" s="8">
+        <v>33</v>
+      </c>
+      <c r="Q3" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="N3" t="s" s="9">
+      <c r="R3" t="s" s="10">
         <v>38</v>
-      </c>
-      <c r="O3" t="s" s="9">
-        <v>38</v>
-      </c>
-      <c r="P3" t="s" s="9">
-        <v>39</v>
-      </c>
-      <c r="Q3" t="s" s="9">
-        <v>36</v>
-      </c>
-      <c r="R3" t="s" s="9">
-        <v>40</v>
-      </c>
-      <c r="S3" t="s" s="11">
-        <v>41</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
     </row>
     <row r="5" ht="20" customHeight="1">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
     </row>
     <row r="6" ht="20" customHeight="1">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
     </row>
     <row r="7" ht="20" customHeight="1">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
     </row>
     <row r="8" ht="20" customHeight="1">
-      <c r="A8" t="s" s="14">
-        <v>42</v>
-      </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
+      <c r="A8" t="s" s="13">
+        <v>39</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
     </row>
     <row r="9" ht="20" customHeight="1">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
     </row>
     <row r="10" ht="20" customHeight="1">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
     </row>
     <row r="11" ht="20" customHeight="1">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
     </row>
     <row r="12" ht="20" customHeight="1">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13"/>
-      <c r="S12" s="13"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
fix(excel): fix device import and export bugs
</commit_message>
<xml_diff>
--- a/server/static/download/templates/devices_template_en.xlsx
+++ b/server/static/download/templates/devices_template_en.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
   <si>
     <t>deviceName</t>
   </si>
@@ -26,9 +26,6 @@
     <t>upLinkSystem</t>
   </si>
   <si>
-    <t>IMEI</t>
-  </si>
-  <si>
     <t>gateway</t>
   </si>
   <si>
@@ -41,6 +38,9 @@
     <t>token</t>
   </si>
   <si>
+    <t>mac</t>
+  </si>
+  <si>
     <t>longitude</t>
   </si>
   <si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>description</t>
-  </si>
-  <si>
-    <t>autoSub</t>
   </si>
   <si>
     <t>device name(unique)</t>
@@ -82,9 +79,6 @@
 Gateway</t>
   </si>
   <si>
-    <t>Required only for LwM2M</t>
-  </si>
-  <si>
     <t>Gateway name,required only for upLinkSystem is gateway</t>
   </si>
   <si>
@@ -94,11 +88,6 @@
     <t>Maximum length 300</t>
   </si>
   <si>
-    <t>Only for LwM2M protocol
-0:no auto subscrie
-1:auto subscribe</t>
-  </si>
-  <si>
     <t>sample row(delete befor import)</t>
   </si>
   <si>
@@ -111,15 +100,15 @@
     <t>Cloud</t>
   </si>
   <si>
-    <t>381787278348467</t>
-  </si>
-  <si>
     <t>sample gateway</t>
   </si>
   <si>
     <t>device12345678</t>
   </si>
   <si>
+    <t>94:17:46:9E:0B:0C</t>
+  </si>
+  <si>
     <t>China</t>
   </si>
   <si>
@@ -130,9 +119,6 @@
   </si>
   <si>
     <t xml:space="preserve">sample row </t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <r>
@@ -288,7 +274,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -361,21 +347,6 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
         <color indexed="10"/>
       </right>
       <top style="thin">
@@ -407,7 +378,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -438,16 +409,13 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1541,7 +1509,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1550,15 +1518,14 @@
     <col min="1" max="1" width="22.3516" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.3516" style="1" customWidth="1"/>
     <col min="3" max="4" width="31" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="1" customWidth="1"/>
-    <col min="6" max="7" width="33" style="1" customWidth="1"/>
-    <col min="8" max="8" width="33.3516" style="1" customWidth="1"/>
-    <col min="9" max="9" width="34.1719" style="1" customWidth="1"/>
+    <col min="5" max="6" width="33" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.3516" style="1" customWidth="1"/>
+    <col min="8" max="9" width="34.1719" style="1" customWidth="1"/>
     <col min="10" max="11" width="16.3516" style="1" customWidth="1"/>
     <col min="12" max="15" width="20.5" style="1" customWidth="1"/>
     <col min="16" max="16" width="21" style="1" customWidth="1"/>
-    <col min="17" max="18" width="16.3516" style="1" customWidth="1"/>
-    <col min="19" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="17" max="17" width="16.3516" style="1" customWidth="1"/>
+    <col min="18" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1574,7 +1541,7 @@
       <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" t="s" s="3">
         <v>4</v>
       </c>
       <c r="F1" t="s" s="3">
@@ -1612,39 +1579,34 @@
       </c>
       <c r="Q1" t="s" s="4">
         <v>16</v>
-      </c>
-      <c r="R1" t="s" s="4">
-        <v>17</v>
       </c>
     </row>
     <row r="2" ht="77" customHeight="1">
       <c r="A2" t="s" s="5">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s" s="5">
         <v>18</v>
       </c>
-      <c r="B2" t="s" s="5">
+      <c r="C2" t="s" s="5">
         <v>19</v>
       </c>
-      <c r="C2" t="s" s="5">
+      <c r="D2" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="D2" t="s" s="5">
+      <c r="E2" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="E2" t="s" s="5">
+      <c r="F2" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="F2" t="s" s="5">
-        <v>23</v>
-      </c>
       <c r="G2" t="s" s="5">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s" s="5">
-        <v>24</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I2" s="5"/>
       <c r="J2" t="s" s="5">
         <v>9</v>
       </c>
@@ -1658,42 +1620,39 @@
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
       <c r="P2" t="s" s="5">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Q2" t="s" s="5">
-        <v>25</v>
-      </c>
-      <c r="R2" t="s" s="5">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="7">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s" s="8">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s" s="8">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s" s="8">
         <v>27</v>
       </c>
-      <c r="B3" t="s" s="8">
+      <c r="E3" t="s" s="8">
         <v>28</v>
       </c>
-      <c r="C3" t="s" s="8">
+      <c r="F3" t="s" s="8">
         <v>29</v>
       </c>
-      <c r="D3" t="s" s="8">
+      <c r="G3" t="s" s="8">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s" s="8">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s" s="8">
         <v>30</v>
-      </c>
-      <c r="E3" t="s" s="8">
-        <v>31</v>
-      </c>
-      <c r="F3" t="s" s="8">
-        <v>32</v>
-      </c>
-      <c r="G3" t="s" s="8">
-        <v>33</v>
-      </c>
-      <c r="H3" t="s" s="8">
-        <v>33</v>
-      </c>
-      <c r="I3" t="s" s="8">
-        <v>33</v>
       </c>
       <c r="J3" s="9">
         <v>116.868765448363</v>
@@ -1702,208 +1661,196 @@
         <v>24.4990810465301</v>
       </c>
       <c r="L3" t="s" s="8">
+        <v>31</v>
+      </c>
+      <c r="M3" t="s" s="8">
+        <v>32</v>
+      </c>
+      <c r="N3" t="s" s="8">
+        <v>32</v>
+      </c>
+      <c r="O3" t="s" s="8">
+        <v>33</v>
+      </c>
+      <c r="P3" t="s" s="8">
+        <v>29</v>
+      </c>
+      <c r="Q3" t="s" s="8">
         <v>34</v>
-      </c>
-      <c r="M3" t="s" s="8">
-        <v>35</v>
-      </c>
-      <c r="N3" t="s" s="8">
-        <v>35</v>
-      </c>
-      <c r="O3" t="s" s="8">
-        <v>36</v>
-      </c>
-      <c r="P3" t="s" s="8">
-        <v>33</v>
-      </c>
-      <c r="Q3" t="s" s="8">
-        <v>37</v>
-      </c>
-      <c r="R3" t="s" s="10">
-        <v>38</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
     </row>
     <row r="5" ht="20" customHeight="1">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
     </row>
     <row r="6" ht="20" customHeight="1">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
     </row>
     <row r="7" ht="20" customHeight="1">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
     </row>
     <row r="8" ht="20" customHeight="1">
-      <c r="A8" t="s" s="13">
-        <v>39</v>
-      </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
+      <c r="A8" t="s" s="12">
+        <v>35</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
     </row>
     <row r="9" ht="20" customHeight="1">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
     </row>
     <row r="10" ht="20" customHeight="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
     </row>
     <row r="11" ht="20" customHeight="1">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
     </row>
     <row r="12" ht="20" customHeight="1">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="12"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>